<commit_message>
adding command line interface
</commit_message>
<xml_diff>
--- a/KineticDatanator/SmilesStuff2.xlsx
+++ b/KineticDatanator/SmilesStuff2.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="1581">
   <si>
-    <t>[c]: PAP + H2O ==&gt; AMP + PI</t>
+    <t>[c]: ATP + DNAD + NH3 ==&gt; NAD + PPI + AMP + H</t>
   </si>
   <si>
     <t>A23CMP</t>
@@ -4887,7 +4887,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4922,7 +4922,7 @@
   <dimension ref="A1:B803"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A790" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A792" activeCellId="0" sqref="A792"/>
+      <selection pane="topLeft" activeCell="A792" activeCellId="1" sqref="A2:B12 A792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>